<commit_message>
added to table s5
</commit_message>
<xml_diff>
--- a/results/supplement/tables/Table_S5.xlsx
+++ b/results/supplement/tables/Table_S5.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Group</t>
   </si>
@@ -33,6 +33,29 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">Raw reads</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">Curated reads</t>
     </r>
     <r>
@@ -44,7 +67,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">1</t>
+      <t xml:space="preserve">2</t>
     </r>
   </si>
   <si>
@@ -67,36 +90,58 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">2</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Streptomycin pretreatment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cefoperazone pretreatment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clindamycin pretreatment</t>
+      <t xml:space="preserve">3</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Streptomycin-pretreatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cefoperazone-pretreatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clindamycin-pretreatment</t>
   </si>
   <si>
     <t xml:space="preserve">ex-Germfree</t>
   </si>
   <si>
-    <t xml:space="preserve">408920*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 = Totals include both paired-end and orphaned reads following quality and adapter trimming</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2 = Mapped and dereplicated read abundances to </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">408920</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1 = Raw paired-end reads from sequencer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 = Totals include both paired-end and orphaned reads following quality and adapter trimming</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3 = Mapped and dereplicated read abundances to </t>
     </r>
     <r>
       <rPr>
@@ -119,7 +164,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">* = Library with RIN score 6.8, caused fewer reads mapped to reference genome</t>
+    <t xml:space="preserve">4 = Library with RIN score 6.8, caused fewer reads mapped to reference genome with no mismatches</t>
   </si>
 </sst>
 </file>
@@ -129,7 +174,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -157,6 +202,14 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -182,7 +235,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -190,6 +243,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -216,28 +276,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -258,17 +322,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -281,83 +346,114 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="n">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>307082142</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>241929815</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="2" t="n">
         <v>8031646</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="n">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>376175754</v>
+      </c>
+      <c r="C3" s="3" t="n">
         <v>317502478</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="D3" s="2" t="n">
         <v>7968641</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="n">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>265973934</v>
+      </c>
+      <c r="C4" s="3" t="n">
         <v>218357990</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="D4" s="2" t="n">
         <v>4659244</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="n">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>320492216</v>
+      </c>
+      <c r="C5" s="3" t="n">
         <v>265361219</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
+  <mergeCells count="4">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:D10"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
typo in read counts
</commit_message>
<xml_diff>
--- a/results/supplement/tables/Table_S5.xlsx
+++ b/results/supplement/tables/Table_S5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Group</t>
   </si>
@@ -43,6 +43,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
     </r>
@@ -79,6 +80,29 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">Mapped reads</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">Final abundances</t>
     </r>
     <r>
@@ -90,7 +114,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">3</t>
+      <t xml:space="preserve">4</t>
     </r>
   </si>
   <si>
@@ -123,25 +147,29 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">4</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">1 = Raw paired-end reads from sequencer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 = Totals include both paired-end and orphaned reads following quality and adapter trimming</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">3 = Mapped and dereplicated read abundances to </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">5</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 = Raw paired-end reads from sequencer, includes all metatranscriptomic reads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 = Totals include both paired-end and orphaned reads following quality and adapter trimming, includes all metatranscriptomic reads</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3 = Mapped reads to </t>
     </r>
     <r>
       <rPr>
@@ -160,19 +188,23 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> strain 630 genome</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">4 = Library with RIN score 6.8, caused fewer reads mapped to reference genome with no mismatches</t>
+      <t xml:space="preserve"> strain 630 genome from Bowtie2 from each pool</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">4 = Read counts after removal of optical + PCR duplicates and normalization to target gene/read length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 = Library with RIN score 6.8, likely caused fewer reads mapped to reference genome with no mismatches</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -210,6 +242,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -276,7 +309,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -297,11 +330,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -322,18 +359,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -349,10 +387,13 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>307082142</v>
@@ -363,10 +404,13 @@
       <c r="D2" s="2" t="n">
         <v>8031646</v>
       </c>
+      <c r="E2" s="2" t="n">
+        <v>299325</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>376175754</v>
@@ -377,10 +421,13 @@
       <c r="D3" s="2" t="n">
         <v>7968641</v>
       </c>
+      <c r="E3" s="2" t="n">
+        <v>222811</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>265973934</v>
@@ -391,10 +438,13 @@
       <c r="D4" s="2" t="n">
         <v>4659244</v>
       </c>
+      <c r="E4" s="2" t="n">
+        <v>108783</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>320492216</v>
@@ -403,57 +453,91 @@
         <v>265361219</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>37829</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="B7" s="5" t="n">
+        <f aca="false">AVERAGE(B2:B5)</f>
+        <v>317431011.5</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <f aca="false">AVERAGE(C2:C5)</f>
+        <v>260787875.5</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <f aca="false">AVERAGE(D2:D5)</f>
+        <v>6886510.33333333</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <f aca="false">AVERAGE(E2:E5)</f>
+        <v>167187</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:D10"/>
+  <mergeCells count="5">
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>